<commit_message>
Update xml and reorder Solution.java
</commit_message>
<xml_diff>
--- a/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
+++ b/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
   <si>
     <t>Замер производительности</t>
   </si>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,8 +856,12 @@
       <c r="G24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -881,8 +885,12 @@
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -906,8 +914,12 @@
       <c r="G26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -931,8 +943,12 @@
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
@@ -956,8 +972,12 @@
       <c r="G28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1003,8 +1023,12 @@
       <c r="F31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -1025,8 +1049,12 @@
       <c r="F32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -1047,8 +1075,12 @@
       <c r="F33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">

</xml_diff>

<commit_message>
Update Home Task Collections.xlsx change 3 answers and write reason in red color
</commit_message>
<xml_diff>
--- a/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
+++ b/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Замер производительности</t>
   </si>
@@ -209,12 +209,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>исправленно</t>
+  </si>
+  <si>
+    <t>Необходимо в случае использования Collections.sort</t>
+  </si>
+  <si>
+    <t>Необходимо для определения уникальности элемента</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +249,27 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -317,7 +340,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -339,6 +362,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,33 +814,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="10"/>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>23</v>
@@ -837,7 +871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -862,11 +896,14 @@
       <c r="H24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -891,11 +928,14 @@
       <c r="H25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -924,7 +964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -953,7 +993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -975,15 +1015,18 @@
       <c r="G28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>46</v>
+      <c r="H28" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>34</v>
@@ -1007,7 +1050,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1033,7 +1076,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Update Table Need hashCode equals
</commit_message>
<xml_diff>
--- a/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
+++ b/Pavel_Vasilev_Collections_Test/Home Task Collections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>Замер производительности</t>
   </si>
@@ -210,13 +210,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>исправленно</t>
-  </si>
-  <si>
-    <t>Необходимо в случае использования Collections.sort</t>
-  </si>
-  <si>
-    <t>Необходимо для определения уникальности элемента</t>
+    <t>+/-</t>
   </si>
 </sst>
 </file>
@@ -258,18 +252,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -340,7 +328,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -365,9 +353,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -671,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,37 +801,33 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>23</v>
@@ -871,7 +854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -897,13 +880,10 @@
         <v>46</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -929,13 +909,10 @@
         <v>46</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -964,7 +941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -987,13 +964,13 @@
         <v>46</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1016,17 +993,14 @@
         <v>46</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>34</v>
@@ -1050,7 +1024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1069,14 +1043,14 @@
       <c r="F31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
+      <c r="G31" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1121,8 +1095,8 @@
       <c r="F33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>45</v>
+      <c r="G33" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>46</v>

</xml_diff>